<commit_message>
Step by step problem solving guide
</commit_message>
<xml_diff>
--- a/electronics-store-sales-analysis/electronics-sales-problem-solving.xlsx
+++ b/electronics-store-sales-analysis/electronics-sales-problem-solving.xlsx
@@ -142,7 +142,7 @@
     <t>Pada masing2 produk tampilkan frekuensi terbeli di tiap bulannya, scatter plot / plot biasa</t>
   </si>
   <si>
-    <t>Pada masing2 produk tampilkan frekuensi terbeli di tiap kotanya, barh plot</t>
+    <t>Pada masing2 produk tampilkan frekuensi terbeli di tiap kotanya, plot biasa</t>
   </si>
   <si>
     <t>Asking and answering questions to the data</t>
@@ -177,10 +177,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;Rp&quot;* #,##0.00_-;\-&quot;Rp&quot;* #,##0.00_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_(* #.##0_);_(* \(#.##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;Rp&quot;* #,##0_-;\-&quot;Rp&quot;* #,##0_-;_-&quot;Rp&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_(* #,###.##000_);_(* \(#,###.##000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -200,14 +200,30 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -221,15 +237,84 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,93 +328,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -358,175 +358,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -680,6 +680,39 @@
       <top/>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -714,39 +747,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -765,8 +765,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -786,148 +786,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1316,8 +1316,8 @@
   <sheetPr/>
   <dimension ref="B2:H52"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="7"/>

</xml_diff>